<commit_message>
General info. New files added to head. First section to Github
</commit_message>
<xml_diff>
--- a/assets/TemplateAsycudaTempMulti.xlsx
+++ b/assets/TemplateAsycudaTempMulti.xlsx
@@ -663,24 +663,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -758,32 +746,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -792,12 +762,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -809,15 +773,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -827,6 +782,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1131,23 +1109,23 @@
   <dimension ref="A1:BB4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25" style="4" customWidth="1"/>
+    <col min="12" max="12" width="25" style="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23.140625" customWidth="1"/>
@@ -1172,574 +1150,574 @@
     <col min="35" max="35" width="30.85546875" customWidth="1"/>
     <col min="36" max="36" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.7109375" style="4" customWidth="1"/>
+    <col min="38" max="38" width="19.7109375" style="1" customWidth="1"/>
     <col min="39" max="39" width="23.42578125" customWidth="1"/>
-    <col min="40" max="40" width="17" style="4" customWidth="1"/>
-    <col min="41" max="41" width="26.140625" style="4" customWidth="1"/>
+    <col min="40" max="40" width="17" style="1" customWidth="1"/>
+    <col min="41" max="41" width="26.140625" style="1" customWidth="1"/>
     <col min="42" max="42" width="15.42578125" customWidth="1"/>
     <col min="43" max="43" width="18" customWidth="1"/>
     <col min="44" max="44" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="17" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="21.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:54" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="8" t="s">
+      <c r="H1" s="15"/>
+      <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="9" t="s">
+      <c r="N1" s="11"/>
+      <c r="O1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="T1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="19"/>
-      <c r="V1" s="9" t="s">
+      <c r="U1" s="9"/>
+      <c r="V1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="8" t="s">
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="18" t="s">
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="18" t="s">
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="9" t="s">
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AJ1" s="18" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="9" t="s">
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AM1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="AN1" s="9" t="s">
+      <c r="AN1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AO1" s="9" t="s">
+      <c r="AO1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AP1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="AR1" s="9" t="s">
+      <c r="AR1" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="AS1" s="9" t="s">
+      <c r="AS1" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="AT1" s="9" t="s">
+      <c r="AT1" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="AU1" s="9" t="s">
+      <c r="AU1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="AV1" s="9" t="s">
+      <c r="AV1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="AW1" s="9" t="s">
+      <c r="AW1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="AX1" s="9" t="s">
+      <c r="AX1" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="AY1" s="9" t="s">
+      <c r="AY1" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="BA1" s="9" t="s">
+      <c r="BA1" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="BB1" s="8" t="s">
+      <c r="BB1" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:54" s="4" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:54" s="1" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AF2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AG2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AH2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AI2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AK2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AL2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AM2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AP2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AR2" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AS2" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AW2" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BB2" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="12" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:54" s="4" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Y3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="Z3" s="12" t="s">
+      <c r="Z3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AB3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AC3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AD3" s="12" t="s">
+      <c r="AD3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AE3" s="12" t="s">
+      <c r="AE3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AF3" s="12" t="s">
+      <c r="AF3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AG3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="AH3" s="12" t="s">
+      <c r="AH3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="AI3" s="12" t="s">
+      <c r="AI3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AJ3" s="12" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AK3" s="12" t="s">
+      <c r="AK3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="AL3" s="13" t="s">
+      <c r="AL3" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="AM3" s="12" t="s">
+      <c r="AM3" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AN3" s="13"/>
-      <c r="AO3" s="13"/>
-      <c r="AP3" s="12" t="s">
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AR3" s="12" t="s">
+      <c r="AR3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AS3" s="12" t="s">
+      <c r="AS3" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AT3" s="13"/>
-      <c r="AU3" s="13"/>
-      <c r="AW3" s="12" t="s">
+      <c r="AT3" s="5"/>
+      <c r="AU3" s="5"/>
+      <c r="AW3" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="AX3" s="13"/>
-      <c r="AY3" s="13"/>
-      <c r="AZ3" s="13"/>
-      <c r="BA3" s="13"/>
-      <c r="BB3" s="12" t="s">
+      <c r="AX3" s="5"/>
+      <c r="AY3" s="5"/>
+      <c r="AZ3" s="5"/>
+      <c r="BA3" s="5"/>
+      <c r="BB3" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="14" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:54" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="20">
         <v>4</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="20">
         <v>1</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="20">
         <v>1</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="6">
         <v>1</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="6">
         <v>9</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="6">
         <v>987654321</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="6">
         <v>0</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U4" s="14" t="s">
+      <c r="U4" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V4" s="14" t="s">
+      <c r="V4" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W4" s="14" t="s">
+      <c r="W4" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="X4" s="14" t="s">
+      <c r="X4" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="Y4" s="14" t="s">
+      <c r="Y4" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="Z4" s="14" t="s">
+      <c r="Z4" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="AA4" s="14" t="s">
+      <c r="AA4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="AB4" s="14" t="b">
+      <c r="AB4" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="AC4" s="14" t="s">
+      <c r="AC4" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AD4" s="14" t="s">
+      <c r="AD4" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AE4" s="14" t="s">
+      <c r="AE4" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="AF4" s="14" t="s">
+      <c r="AF4" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="AG4" s="14" t="s">
+      <c r="AG4" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AH4" s="14">
+      <c r="AH4" s="6">
         <v>6000</v>
       </c>
-      <c r="AI4" s="14">
+      <c r="AI4" s="6">
         <v>136.54</v>
       </c>
-      <c r="AJ4" s="14">
+      <c r="AJ4" s="6">
         <v>1</v>
       </c>
-      <c r="AK4" s="14">
+      <c r="AK4" s="6">
         <v>2</v>
       </c>
-      <c r="AL4" s="17">
+      <c r="AL4" s="7">
         <v>32</v>
       </c>
-      <c r="AM4" s="14">
+      <c r="AM4" s="6">
         <v>32</v>
       </c>
-      <c r="AN4" s="17"/>
-      <c r="AO4" s="17"/>
-      <c r="AP4" s="14" t="s">
+      <c r="AN4" s="7"/>
+      <c r="AO4" s="7"/>
+      <c r="AP4" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AR4" s="14" t="s">
+      <c r="AR4" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AS4" s="14" t="s">
+      <c r="AS4" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AT4" s="17"/>
-      <c r="AU4" s="17"/>
-      <c r="AW4" s="14" t="s">
+      <c r="AT4" s="7"/>
+      <c r="AU4" s="7"/>
+      <c r="AW4" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AX4" s="17"/>
-      <c r="AY4" s="17"/>
-      <c r="AZ4" s="17"/>
-      <c r="BA4" s="17"/>
-      <c r="BB4" s="14" t="s">
+      <c r="AX4" s="7"/>
+      <c r="AY4" s="7"/>
+      <c r="AZ4" s="7"/>
+      <c r="BA4" s="7"/>
+      <c r="BB4" s="6" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="AC1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AG1:AH1"/>
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1779,224 +1757,224 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="8" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="8" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="24"/>
-      <c r="N1" s="9" t="s">
+      <c r="M1" s="11"/>
+      <c r="N1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="T1" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="U1" s="19"/>
+      <c r="U1" s="9"/>
     </row>
     <row r="2" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4" t="s">
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4" t="s">
+      <c r="S2" s="1"/>
+      <c r="T2" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12" t="s">
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12" t="s">
+      <c r="S3" s="4"/>
+      <c r="T3" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="4" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="6">
         <v>9</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="6">
         <v>10019120</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14" t="s">
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14" t="s">
+      <c r="S4" s="6"/>
+      <c r="T4" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="U4" s="14" t="s">
+      <c r="U4" s="6" t="s">
         <v>198</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Done with the single item. Feel hopeful
</commit_message>
<xml_diff>
--- a/assets/TemplateAsycudaTempMulti.xlsx
+++ b/assets/TemplateAsycudaTempMulti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="23955" windowHeight="4695" tabRatio="366"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="23955" windowHeight="4695" tabRatio="366" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="215">
   <si>
     <t>Type Decl.</t>
   </si>
@@ -259,9 +259,6 @@
   </si>
   <si>
     <t>Transport-&gt;Means_of_transport-&gt;Border_information-&gt;Nationality</t>
-  </si>
-  <si>
-    <t>22*** Mon &amp; shuma totale ne fature (jo sh i sigurt)</t>
   </si>
   <si>
     <t>Valuation-&gt;Gs_Invoice-&gt;Currency_code</t>
@@ -626,13 +623,52 @@
   </si>
   <si>
     <t>Alban Shehri</t>
+  </si>
+  <si>
+    <t>22*** Mon &amp; shuma totale ne fature</t>
+  </si>
+  <si>
+    <t>Net_weight_itm</t>
+  </si>
+  <si>
+    <t>Total_cost_itm</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Total_CIF_itm</t>
+  </si>
+  <si>
+    <t>819240</t>
+  </si>
+  <si>
+    <t>Rate_of_adjustement</t>
+  </si>
+  <si>
+    <t>Statistical_value</t>
+  </si>
+  <si>
+    <t>Amount_national_currency</t>
+  </si>
+  <si>
+    <t>Amount_foreign_currency</t>
+  </si>
+  <si>
+    <t>6000</t>
+  </si>
+  <si>
+    <t>Currency_code</t>
+  </si>
+  <si>
+    <t>Valuation_item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,6 +697,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -746,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -767,30 +809,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -805,6 +823,34 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1108,20 +1154,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -1170,22 +1216,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="15"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1198,10 +1244,10 @@
       <c r="L1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="11"/>
+      <c r="N1" s="18"/>
       <c r="O1" s="3" t="s">
         <v>37</v>
       </c>
@@ -1217,10 +1263,10 @@
       <c r="S1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="9"/>
+      <c r="U1" s="20"/>
       <c r="V1" s="3" t="s">
         <v>53</v>
       </c>
@@ -1233,107 +1279,107 @@
       <c r="Y1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="AA1" s="9"/>
+      <c r="AA1" s="20"/>
       <c r="AB1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="8" t="s">
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH1" s="9"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="AH1" s="20"/>
       <c r="AI1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AJ1" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="AK1" s="9"/>
+        <v>85</v>
+      </c>
+      <c r="AJ1" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK1" s="20"/>
       <c r="AL1" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AM1" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AN1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AO1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="AP1" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="AQ1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AR1" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AS1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AT1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AU1" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="AW1" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="AX1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AY1" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BB1" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:54" s="1" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -1403,65 +1449,65 @@
         <v>80</v>
       </c>
       <c r="AG2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="AI2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AJ2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AK2" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="AL2" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:54" s="4" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -1531,25 +1577,25 @@
         <v>69</v>
       </c>
       <c r="AG3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="AH3" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="AI3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AJ3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AK3" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="AL3" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AM3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AN3" s="5"/>
       <c r="AO3" s="5"/>
@@ -1557,45 +1603,45 @@
         <v>76</v>
       </c>
       <c r="AR3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AS3" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
       <c r="AW3" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AX3" s="5"/>
       <c r="AY3" s="5"/>
       <c r="AZ3" s="5"/>
       <c r="BA3" s="5"/>
       <c r="BB3" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:54" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="12">
+        <v>4</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="20">
-        <v>4</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20" t="s">
+      <c r="E4" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="F4" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="G4" s="20">
+      <c r="G4" s="12">
         <v>1</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="12">
         <v>1</v>
       </c>
       <c r="J4" s="6">
@@ -1605,64 +1651,64 @@
         <v>9</v>
       </c>
       <c r="L4" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="N4" s="6">
         <v>987654321</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R4" s="6">
         <v>0</v>
       </c>
       <c r="T4" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="U4" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="V4" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="W4" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y4" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W4" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y4" s="6" t="s">
+      <c r="Z4" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="Z4" s="6" t="s">
+      <c r="AA4" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="AB4" s="6" t="b">
         <v>0</v>
       </c>
       <c r="AC4" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD4" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AD4" s="6" t="s">
+      <c r="AE4" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG4" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="AE4" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG4" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="AH4" s="6">
         <v>6000</v>
@@ -1685,39 +1731,39 @@
       <c r="AN4" s="7"/>
       <c r="AO4" s="7"/>
       <c r="AP4" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AR4" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="AS4" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="AS4" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="AT4" s="7"/>
       <c r="AU4" s="7"/>
       <c r="AW4" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AX4" s="7"/>
       <c r="AY4" s="7"/>
       <c r="AZ4" s="7"/>
       <c r="BA4" s="7"/>
       <c r="BB4" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1726,10 +1772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,199 +1789,256 @@
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.28515625" customWidth="1"/>
+    <col min="11" max="18" width="33.42578125" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="11"/>
+      <c r="G1" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="18"/>
       <c r="I1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="O1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="U1" s="18"/>
+      <c r="V1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB1" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="T1" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="U1" s="9"/>
+      <c r="AC1" s="20"/>
     </row>
-    <row r="2" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="I2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="R2" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="S3" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="T3" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="U3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="V3" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1" t="s">
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="U2" s="1" t="s">
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="AC3" s="4" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="F4" s="6">
         <v>1</v>
@@ -1944,48 +2047,73 @@
         <v>10019120</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J4" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="O4" s="23">
+        <v>815580</v>
+      </c>
+      <c r="P4" s="23">
+        <v>815580</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="S4" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="T4" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="U4" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="V4" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="N4" s="6" t="s">
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6" t="s">
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6" t="s">
+      <c r="AC4" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="L1:M1"/>
     <mergeCell ref="T1:U1"/>
+    <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>